<commit_message>
Scrape Current Makert Data
</commit_message>
<xml_diff>
--- a/getNseMarketData/parameterfile/MarketData.xlsx
+++ b/getNseMarketData/parameterfile/MarketData.xlsx
@@ -8,12 +8,46 @@
   </bookViews>
   <sheets>
     <sheet name="MarketData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="List of Available Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>nobin thomas</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>nobin thomas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Static Colmns.Update the next colmn headers to fetch the required data</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="125">
   <si>
@@ -396,7 +430,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,8 +566,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -711,6 +758,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -874,10 +927,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1215,7 +1269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1224,28 +1280,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -1669,6 +1725,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1676,7 +1733,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>

</xml_diff>